<commit_message>
fix some bugs and add id to the campagne
</commit_message>
<xml_diff>
--- a/config-evaluation-froid.xlsx
+++ b/config-evaluation-froid.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mehdi\OneDrive\Documents\BCP\evaluation-froid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4EEC662-53C6-4C39-86BB-FD6D25991C1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{441EA0CF-408B-4F3B-9594-973FD295CA95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="23">
   <si>
     <t>MATRICULE</t>
   </si>
@@ -82,6 +82,18 @@
   </si>
   <si>
     <t>LAARAJ</t>
+  </si>
+  <si>
+    <t>MABROUK</t>
+  </si>
+  <si>
+    <t>WAFAE</t>
+  </si>
+  <si>
+    <t>YOUSSEFI</t>
+  </si>
+  <si>
+    <t>ABDELMALEK</t>
   </si>
 </sst>
 </file>
@@ -417,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -534,6 +546,38 @@
         <v>36547</v>
       </c>
     </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>7573</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4">
+        <v>7373</v>
+      </c>
+      <c r="H4" t="s">
+        <v>19</v>
+      </c>
+      <c r="I4" t="s">
+        <v>20</v>
+      </c>
+      <c r="J4" s="2">
+        <v>35802</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>